<commit_message>
Üzerine yazılan Excel'deki detay hatalar ayıklandı.
</commit_message>
<xml_diff>
--- a/FR_02_MT.xlsx
+++ b/FR_02_MT.xlsx
@@ -1753,7 +1753,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1766,12 +1766,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1784,31 +1778,289 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1829,358 +2081,73 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2240,7 +2207,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:colOff>255436</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>198544</xdr:rowOff>
     </xdr:to>
@@ -2363,8 +2330,8 @@
           <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>257175</xdr:colOff>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>25262</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:to>
@@ -2427,8 +2394,8 @@
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>15</xdr:col>
-          <xdr:colOff>542925</xdr:colOff>
+          <xdr:col>16</xdr:col>
+          <xdr:colOff>37686</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>133350</xdr:rowOff>
         </xdr:to>
@@ -2742,10 +2709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB429"/>
+  <dimension ref="A1:AE429"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U41" sqref="U41:Y41"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AD34" sqref="AD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2755,860 +2722,861 @@
     <col min="4" max="4" width="0.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="0.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="3.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="3.28515625" style="2" customWidth="1"/>
     <col min="9" max="9" width="5.5703125" style="2" customWidth="1"/>
     <col min="10" max="10" width="3.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" style="2" customWidth="1"/>
     <col min="12" max="12" width="4.85546875" style="2" customWidth="1"/>
-    <col min="13" max="15" width="0.85546875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="3.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="0.140625" style="2" customWidth="1"/>
+    <col min="14" max="15" width="0.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="2.85546875" style="2" customWidth="1"/>
     <col min="18" max="18" width="10.7109375" style="2" customWidth="1"/>
     <col min="19" max="19" width="4.85546875" style="2" customWidth="1"/>
     <col min="20" max="20" width="3.85546875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="3.42578125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="0.85546875" style="2" customWidth="1"/>
+    <col min="21" max="21" width="2.42578125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="0.28515625" style="2" customWidth="1"/>
     <col min="23" max="23" width="10.7109375" style="2" customWidth="1"/>
     <col min="24" max="24" width="2.42578125" style="2" customWidth="1"/>
-    <col min="25" max="25" width="5.7109375" style="2" customWidth="1"/>
+    <col min="25" max="25" width="3.85546875" style="2" customWidth="1"/>
     <col min="26" max="26" width="4.7109375" style="2" customWidth="1"/>
     <col min="27" max="27" width="6.7109375" style="2" customWidth="1"/>
-    <col min="28" max="28" width="7.85546875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="7.140625" style="2" customWidth="1"/>
     <col min="29" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="125"/>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="131" t="s">
+      <c r="A1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132"/>
-      <c r="N1" s="132"/>
-      <c r="O1" s="132"/>
-      <c r="P1" s="132"/>
-      <c r="Q1" s="132"/>
-      <c r="R1" s="132"/>
-      <c r="S1" s="132"/>
-      <c r="T1" s="132"/>
-      <c r="U1" s="132"/>
-      <c r="V1" s="132"/>
-      <c r="W1" s="132"/>
-      <c r="X1" s="132"/>
-      <c r="Y1" s="132"/>
-      <c r="Z1" s="132"/>
-      <c r="AA1" s="132"/>
-      <c r="AB1" s="133"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="14"/>
     </row>
     <row r="2" spans="1:28" ht="43.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="128"/>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="130"/>
-      <c r="H2" s="134" t="s">
+      <c r="A2" s="124"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="135"/>
-      <c r="L2" s="135"/>
-      <c r="M2" s="135"/>
-      <c r="N2" s="135"/>
-      <c r="O2" s="135"/>
-      <c r="P2" s="135"/>
-      <c r="Q2" s="135"/>
-      <c r="R2" s="135"/>
-      <c r="S2" s="135"/>
-      <c r="T2" s="135"/>
-      <c r="U2" s="135"/>
-      <c r="V2" s="135"/>
-      <c r="W2" s="135"/>
-      <c r="X2" s="135"/>
-      <c r="Y2" s="135"/>
-      <c r="Z2" s="135"/>
-      <c r="AA2" s="135"/>
-      <c r="AB2" s="136"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="17"/>
     </row>
     <row r="3" spans="1:28" s="4" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="138"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="140"/>
-      <c r="M3" s="140"/>
-      <c r="N3" s="140"/>
-      <c r="O3" s="140"/>
-      <c r="P3" s="140"/>
-      <c r="Q3" s="141" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="138"/>
-      <c r="S3" s="138"/>
-      <c r="T3" s="142"/>
-      <c r="U3" s="142"/>
-      <c r="V3" s="142"/>
-      <c r="W3" s="142"/>
-      <c r="X3" s="141" t="s">
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="Y3" s="138"/>
-      <c r="Z3" s="138"/>
-      <c r="AA3" s="143"/>
-      <c r="AB3" s="144"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="24"/>
+      <c r="AB3" s="25"/>
     </row>
     <row r="4" spans="1:28" s="4" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="117"/>
-      <c r="C4" s="117"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="118"/>
-      <c r="H4" s="118"/>
-      <c r="I4" s="118"/>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="118"/>
-      <c r="M4" s="118"/>
-      <c r="N4" s="118"/>
-      <c r="O4" s="118"/>
-      <c r="P4" s="118"/>
-      <c r="Q4" s="41" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="117"/>
-      <c r="S4" s="117"/>
-      <c r="T4" s="123"/>
-      <c r="U4" s="124"/>
-      <c r="V4" s="124"/>
-      <c r="W4" s="124"/>
-      <c r="X4" s="41" t="s">
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="35"/>
+      <c r="V4" s="35"/>
+      <c r="W4" s="35"/>
+      <c r="X4" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="Y4" s="117"/>
-      <c r="Z4" s="117"/>
-      <c r="AA4" s="120"/>
-      <c r="AB4" s="121"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="33"/>
     </row>
     <row r="5" spans="1:28" s="4" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="117"/>
-      <c r="C5" s="117"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
-      <c r="I5" s="118"/>
-      <c r="J5" s="118"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="118"/>
-      <c r="M5" s="118"/>
-      <c r="N5" s="118"/>
-      <c r="O5" s="118"/>
-      <c r="P5" s="118"/>
-      <c r="Q5" s="41" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="R5" s="117"/>
-      <c r="S5" s="117"/>
-      <c r="T5" s="119"/>
-      <c r="U5" s="119"/>
-      <c r="V5" s="119"/>
-      <c r="W5" s="119"/>
-      <c r="X5" s="41" t="s">
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="Y5" s="117"/>
-      <c r="Z5" s="117"/>
-      <c r="AA5" s="122"/>
-      <c r="AB5" s="121"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="27"/>
+      <c r="AA5" s="32"/>
+      <c r="AB5" s="33"/>
     </row>
     <row r="6" spans="1:28" s="4" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="117"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="118"/>
-      <c r="K6" s="118"/>
-      <c r="L6" s="118"/>
-      <c r="M6" s="118"/>
-      <c r="N6" s="118"/>
-      <c r="O6" s="118"/>
-      <c r="P6" s="118"/>
-      <c r="Q6" s="41" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="117"/>
-      <c r="S6" s="117"/>
-      <c r="T6" s="119"/>
-      <c r="U6" s="119"/>
-      <c r="V6" s="119"/>
-      <c r="W6" s="119"/>
-      <c r="X6" s="41" t="s">
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="Y6" s="117"/>
-      <c r="Z6" s="117"/>
-      <c r="AA6" s="120"/>
-      <c r="AB6" s="121"/>
+      <c r="Y6" s="27"/>
+      <c r="Z6" s="27"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6" s="33"/>
     </row>
     <row r="7" spans="1:28" s="4" customFormat="1" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="113"/>
-      <c r="C7" s="113"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="114"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="114"/>
-      <c r="H7" s="114"/>
-      <c r="I7" s="114"/>
-      <c r="J7" s="114"/>
-      <c r="K7" s="114"/>
-      <c r="L7" s="114"/>
-      <c r="M7" s="114"/>
-      <c r="N7" s="114"/>
-      <c r="O7" s="114"/>
-      <c r="P7" s="114"/>
-      <c r="Q7" s="37" t="s">
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="R7" s="113"/>
-      <c r="S7" s="113"/>
-      <c r="T7" s="115"/>
-      <c r="U7" s="115"/>
-      <c r="V7" s="115"/>
-      <c r="W7" s="115"/>
-      <c r="X7" s="37" t="s">
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="Y7" s="113"/>
-      <c r="Z7" s="113"/>
-      <c r="AA7" s="114"/>
-      <c r="AB7" s="116"/>
+      <c r="Y7" s="37"/>
+      <c r="Z7" s="37"/>
+      <c r="AA7" s="38"/>
+      <c r="AB7" s="41"/>
     </row>
     <row r="8" spans="1:28" s="4" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="110" t="s">
+      <c r="A8" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="111"/>
-      <c r="C8" s="111"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="111"/>
-      <c r="F8" s="111"/>
-      <c r="G8" s="111"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="111"/>
-      <c r="J8" s="111"/>
-      <c r="K8" s="111"/>
-      <c r="L8" s="111"/>
-      <c r="M8" s="111"/>
-      <c r="N8" s="111"/>
-      <c r="O8" s="111"/>
-      <c r="P8" s="111"/>
-      <c r="Q8" s="111"/>
-      <c r="R8" s="111"/>
-      <c r="S8" s="111"/>
-      <c r="T8" s="111"/>
-      <c r="U8" s="111"/>
-      <c r="V8" s="111"/>
-      <c r="W8" s="111"/>
-      <c r="X8" s="111"/>
-      <c r="Y8" s="111"/>
-      <c r="Z8" s="111"/>
-      <c r="AA8" s="111"/>
-      <c r="AB8" s="112"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="44"/>
+      <c r="V8" s="44"/>
+      <c r="W8" s="44"/>
+      <c r="X8" s="44"/>
+      <c r="Y8" s="44"/>
+      <c r="Z8" s="44"/>
+      <c r="AA8" s="44"/>
+      <c r="AB8" s="45"/>
     </row>
     <row r="9" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="41" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="45"/>
-      <c r="U9" s="45"/>
-      <c r="V9" s="45"/>
-      <c r="W9" s="41" t="s">
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="42"/>
+      <c r="V9" s="42"/>
+      <c r="W9" s="111" t="s">
         <v>43</v>
       </c>
-      <c r="X9" s="41"/>
-      <c r="Y9" s="41"/>
-      <c r="Z9" s="45"/>
-      <c r="AA9" s="45"/>
+      <c r="X9" s="111"/>
+      <c r="Y9" s="111"/>
+      <c r="Z9" s="42"/>
+      <c r="AA9" s="42"/>
       <c r="AB9" s="46"/>
     </row>
     <row r="10" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="41" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="45"/>
-      <c r="R10" s="45"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="45"/>
-      <c r="U10" s="45"/>
-      <c r="V10" s="45"/>
-      <c r="W10" s="44" t="s">
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="42"/>
+      <c r="U10" s="42"/>
+      <c r="V10" s="42"/>
+      <c r="W10" s="111" t="s">
         <v>44</v>
       </c>
-      <c r="X10" s="44"/>
-      <c r="Y10" s="44"/>
-      <c r="Z10" s="45"/>
-      <c r="AA10" s="45"/>
+      <c r="X10" s="111"/>
+      <c r="Y10" s="111"/>
+      <c r="Z10" s="42"/>
+      <c r="AA10" s="42"/>
       <c r="AB10" s="46"/>
     </row>
-    <row r="11" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
+    <row r="11" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="41" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="45"/>
-      <c r="U11" s="45"/>
-      <c r="V11" s="45"/>
-      <c r="W11" s="44"/>
-      <c r="X11" s="44"/>
-      <c r="Y11" s="44"/>
-      <c r="Z11" s="45"/>
-      <c r="AA11" s="45"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="42"/>
+      <c r="V11" s="42"/>
+      <c r="W11" s="111"/>
+      <c r="X11" s="111"/>
+      <c r="Y11" s="111"/>
+      <c r="Z11" s="42"/>
+      <c r="AA11" s="42"/>
       <c r="AB11" s="46"/>
     </row>
-    <row r="12" spans="1:28" s="10" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
+    <row r="12" spans="1:28" s="8" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="41" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="101"/>
+      <c r="F12" s="101"/>
+      <c r="G12" s="101"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="101"/>
+      <c r="J12" s="101"/>
+      <c r="K12" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="34"/>
-      <c r="S12" s="34"/>
-      <c r="T12" s="34"/>
-      <c r="U12" s="34"/>
-      <c r="V12" s="34"/>
-      <c r="W12" s="41" t="s">
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="101"/>
+      <c r="R12" s="101"/>
+      <c r="S12" s="101"/>
+      <c r="T12" s="101"/>
+      <c r="U12" s="101"/>
+      <c r="V12" s="101"/>
+      <c r="W12" s="111" t="s">
         <v>54</v>
       </c>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="33"/>
-      <c r="AA12" s="34"/>
-      <c r="AB12" s="35"/>
+      <c r="X12" s="111"/>
+      <c r="Y12" s="111"/>
+      <c r="Z12" s="100"/>
+      <c r="AA12" s="101"/>
+      <c r="AB12" s="102"/>
     </row>
-    <row r="13" spans="1:28" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="40" t="s">
+    <row r="13" spans="1:28" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="41" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="45"/>
-      <c r="V13" s="45"/>
-      <c r="W13" s="15" t="s">
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="42"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="42"/>
+      <c r="V13" s="42"/>
+      <c r="W13" s="112" t="s">
         <v>63</v>
       </c>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="17"/>
-      <c r="Z13" s="21"/>
-      <c r="AA13" s="22"/>
-      <c r="AB13" s="23"/>
+      <c r="X13" s="113"/>
+      <c r="Y13" s="114"/>
+      <c r="Z13" s="105"/>
+      <c r="AA13" s="106"/>
+      <c r="AB13" s="107"/>
     </row>
-    <row r="14" spans="1:28" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="37" t="s">
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="103"/>
+      <c r="I14" s="103"/>
+      <c r="J14" s="103"/>
+      <c r="K14" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="39"/>
-      <c r="S14" s="39"/>
-      <c r="T14" s="39"/>
-      <c r="U14" s="39"/>
-      <c r="V14" s="39"/>
-      <c r="W14" s="18" t="s">
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="104"/>
+      <c r="T14" s="104"/>
+      <c r="U14" s="104"/>
+      <c r="V14" s="104"/>
+      <c r="W14" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="X14" s="19"/>
-      <c r="Y14" s="20"/>
-      <c r="Z14" s="24"/>
-      <c r="AA14" s="25"/>
-      <c r="AB14" s="26"/>
+      <c r="X14" s="116"/>
+      <c r="Y14" s="117"/>
+      <c r="Z14" s="108"/>
+      <c r="AA14" s="109"/>
+      <c r="AB14" s="110"/>
     </row>
     <row r="15" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="96"/>
-      <c r="B15" s="97"/>
-      <c r="C15" s="97"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="97"/>
-      <c r="G15" s="97"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="99"/>
-      <c r="J15" s="99"/>
-      <c r="K15" s="99"/>
-      <c r="L15" s="99"/>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99"/>
-      <c r="P15" s="100"/>
-      <c r="Q15" s="107" t="s">
+      <c r="A15" s="53"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="57"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="118" t="s">
         <v>55</v>
       </c>
-      <c r="R15" s="108"/>
-      <c r="S15" s="108"/>
-      <c r="T15" s="108"/>
-      <c r="U15" s="108"/>
-      <c r="V15" s="108"/>
-      <c r="W15" s="108"/>
-      <c r="X15" s="108"/>
-      <c r="Y15" s="108"/>
-      <c r="Z15" s="108"/>
-      <c r="AA15" s="108"/>
-      <c r="AB15" s="109"/>
+      <c r="R15" s="119"/>
+      <c r="S15" s="119"/>
+      <c r="T15" s="119"/>
+      <c r="U15" s="119"/>
+      <c r="V15" s="119"/>
+      <c r="W15" s="119"/>
+      <c r="X15" s="119"/>
+      <c r="Y15" s="119"/>
+      <c r="Z15" s="119"/>
+      <c r="AA15" s="119"/>
+      <c r="AB15" s="120"/>
     </row>
     <row r="16" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="98"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="101"/>
-      <c r="I16" s="101"/>
-      <c r="J16" s="101"/>
-      <c r="K16" s="101"/>
-      <c r="L16" s="101"/>
-      <c r="M16" s="101"/>
-      <c r="N16" s="101"/>
-      <c r="O16" s="101"/>
-      <c r="P16" s="102"/>
-      <c r="Q16" s="103" t="s">
+      <c r="A16" s="55"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="59"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="R16" s="104"/>
-      <c r="S16" s="90" t="s">
+      <c r="R16" s="62"/>
+      <c r="S16" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="T16" s="90"/>
-      <c r="U16" s="90"/>
-      <c r="V16" s="90"/>
-      <c r="W16" s="90"/>
-      <c r="X16" s="90"/>
-      <c r="Y16" s="90"/>
-      <c r="Z16" s="90"/>
-      <c r="AA16" s="90"/>
-      <c r="AB16" s="91"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="47"/>
+      <c r="V16" s="47"/>
+      <c r="W16" s="47"/>
+      <c r="X16" s="47"/>
+      <c r="Y16" s="47"/>
+      <c r="Z16" s="47"/>
+      <c r="AA16" s="47"/>
+      <c r="AB16" s="48"/>
     </row>
     <row r="17" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="98"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="101"/>
-      <c r="I17" s="101"/>
-      <c r="J17" s="101"/>
-      <c r="K17" s="101"/>
-      <c r="L17" s="101"/>
-      <c r="M17" s="101"/>
-      <c r="N17" s="101"/>
-      <c r="O17" s="101"/>
-      <c r="P17" s="102"/>
-      <c r="Q17" s="105" t="s">
+      <c r="A17" s="55"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="59"/>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="R17" s="104"/>
-      <c r="S17" s="106" t="s">
+      <c r="R17" s="62"/>
+      <c r="S17" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="T17" s="90"/>
-      <c r="U17" s="90"/>
-      <c r="V17" s="90"/>
-      <c r="W17" s="90"/>
-      <c r="X17" s="90"/>
-      <c r="Y17" s="90"/>
-      <c r="Z17" s="90"/>
-      <c r="AA17" s="90"/>
-      <c r="AB17" s="91"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="47"/>
+      <c r="V17" s="47"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="47"/>
+      <c r="Y17" s="47"/>
+      <c r="Z17" s="47"/>
+      <c r="AA17" s="47"/>
+      <c r="AB17" s="48"/>
     </row>
     <row r="18" spans="1:28" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="98"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="101"/>
-      <c r="I18" s="101"/>
-      <c r="J18" s="101"/>
-      <c r="K18" s="101"/>
-      <c r="L18" s="101"/>
-      <c r="M18" s="101"/>
-      <c r="N18" s="101"/>
-      <c r="O18" s="101"/>
-      <c r="P18" s="102"/>
-      <c r="Q18" s="105" t="s">
+      <c r="A18" s="55"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="59"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="R18" s="104"/>
-      <c r="S18" s="90" t="s">
+      <c r="R18" s="62"/>
+      <c r="S18" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="T18" s="90"/>
-      <c r="U18" s="90"/>
-      <c r="V18" s="90"/>
-      <c r="W18" s="90"/>
-      <c r="X18" s="90"/>
-      <c r="Y18" s="90"/>
-      <c r="Z18" s="90"/>
-      <c r="AA18" s="90"/>
-      <c r="AB18" s="91"/>
+      <c r="T18" s="47"/>
+      <c r="U18" s="47"/>
+      <c r="V18" s="47"/>
+      <c r="W18" s="47"/>
+      <c r="X18" s="47"/>
+      <c r="Y18" s="47"/>
+      <c r="Z18" s="47"/>
+      <c r="AA18" s="47"/>
+      <c r="AB18" s="48"/>
     </row>
     <row r="19" spans="1:28" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="98"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="101"/>
-      <c r="I19" s="101"/>
-      <c r="J19" s="101"/>
-      <c r="K19" s="101"/>
-      <c r="L19" s="101"/>
-      <c r="M19" s="101"/>
-      <c r="N19" s="101"/>
-      <c r="O19" s="101"/>
-      <c r="P19" s="102"/>
-      <c r="Q19" s="92" t="s">
+      <c r="A19" s="55"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="R19" s="93"/>
-      <c r="S19" s="94" t="s">
+      <c r="R19" s="50"/>
+      <c r="S19" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="T19" s="94"/>
-      <c r="U19" s="94"/>
-      <c r="V19" s="94"/>
-      <c r="W19" s="94"/>
-      <c r="X19" s="94"/>
-      <c r="Y19" s="94"/>
-      <c r="Z19" s="94"/>
-      <c r="AA19" s="94"/>
-      <c r="AB19" s="95"/>
+      <c r="T19" s="51"/>
+      <c r="U19" s="51"/>
+      <c r="V19" s="51"/>
+      <c r="W19" s="51"/>
+      <c r="X19" s="51"/>
+      <c r="Y19" s="51"/>
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="51"/>
+      <c r="AB19" s="52"/>
     </row>
     <row r="20" spans="1:28" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="77" t="s">
+      <c r="A20" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="78"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="78"/>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="79"/>
-      <c r="I20" s="79"/>
-      <c r="J20" s="79"/>
-      <c r="K20" s="79"/>
-      <c r="L20" s="79"/>
-      <c r="M20" s="79"/>
-      <c r="N20" s="79"/>
-      <c r="O20" s="79"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="80"/>
-      <c r="R20" s="80"/>
-      <c r="S20" s="80"/>
-      <c r="T20" s="80"/>
-      <c r="U20" s="80"/>
-      <c r="V20" s="80"/>
-      <c r="W20" s="80"/>
-      <c r="X20" s="80"/>
-      <c r="Y20" s="80"/>
-      <c r="Z20" s="80"/>
-      <c r="AA20" s="80"/>
-      <c r="AB20" s="81"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="75"/>
+      <c r="M20" s="75"/>
+      <c r="N20" s="75"/>
+      <c r="O20" s="75"/>
+      <c r="P20" s="75"/>
+      <c r="Q20" s="76"/>
+      <c r="R20" s="76"/>
+      <c r="S20" s="76"/>
+      <c r="T20" s="76"/>
+      <c r="U20" s="76"/>
+      <c r="V20" s="76"/>
+      <c r="W20" s="76"/>
+      <c r="X20" s="76"/>
+      <c r="Y20" s="76"/>
+      <c r="Z20" s="76"/>
+      <c r="AA20" s="76"/>
+      <c r="AB20" s="77"/>
     </row>
     <row r="21" spans="1:28" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="82" t="s">
+      <c r="A21" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="83"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="85"/>
-      <c r="J21" s="85"/>
-      <c r="K21" s="85"/>
-      <c r="L21" s="85"/>
-      <c r="M21" s="85"/>
-      <c r="N21" s="85"/>
-      <c r="O21" s="85"/>
-      <c r="P21" s="85"/>
-      <c r="Q21" s="85"/>
-      <c r="R21" s="85"/>
-      <c r="S21" s="85"/>
-      <c r="T21" s="85"/>
-      <c r="U21" s="85"/>
-      <c r="V21" s="85"/>
-      <c r="W21" s="85"/>
-      <c r="X21" s="85"/>
-      <c r="Y21" s="85"/>
-      <c r="Z21" s="85"/>
-      <c r="AA21" s="85"/>
-      <c r="AB21" s="86"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="81"/>
+      <c r="M21" s="81"/>
+      <c r="N21" s="81"/>
+      <c r="O21" s="81"/>
+      <c r="P21" s="81"/>
+      <c r="Q21" s="81"/>
+      <c r="R21" s="81"/>
+      <c r="S21" s="81"/>
+      <c r="T21" s="81"/>
+      <c r="U21" s="81"/>
+      <c r="V21" s="81"/>
+      <c r="W21" s="81"/>
+      <c r="X21" s="81"/>
+      <c r="Y21" s="81"/>
+      <c r="Z21" s="81"/>
+      <c r="AA21" s="81"/>
+      <c r="AB21" s="82"/>
     </row>
     <row r="22" spans="1:28" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="87" t="s">
+      <c r="A22" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="88"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="88"/>
-      <c r="F22" s="88"/>
-      <c r="G22" s="88"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="71"/>
-      <c r="N22" s="71"/>
-      <c r="O22" s="71"/>
-      <c r="P22" s="71"/>
-      <c r="Q22" s="71"/>
-      <c r="R22" s="71"/>
-      <c r="S22" s="71"/>
-      <c r="T22" s="71"/>
-      <c r="U22" s="71"/>
-      <c r="V22" s="71"/>
-      <c r="W22" s="71"/>
-      <c r="X22" s="71"/>
-      <c r="Y22" s="71"/>
-      <c r="Z22" s="71"/>
-      <c r="AA22" s="71"/>
-      <c r="AB22" s="89"/>
+      <c r="B22" s="84"/>
+      <c r="C22" s="84"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="127"/>
+      <c r="I22" s="127"/>
+      <c r="J22" s="127"/>
+      <c r="K22" s="127"/>
+      <c r="L22" s="127"/>
+      <c r="M22" s="127"/>
+      <c r="N22" s="127"/>
+      <c r="O22" s="127"/>
+      <c r="P22" s="127"/>
+      <c r="Q22" s="127"/>
+      <c r="R22" s="127"/>
+      <c r="S22" s="127"/>
+      <c r="T22" s="127"/>
+      <c r="U22" s="127"/>
+      <c r="V22" s="127"/>
+      <c r="W22" s="127"/>
+      <c r="X22" s="127"/>
+      <c r="Y22" s="127"/>
+      <c r="Z22" s="127"/>
+      <c r="AA22" s="127"/>
+      <c r="AB22" s="128"/>
     </row>
     <row r="23" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="72" t="s">
+      <c r="A23" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="61"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="61"/>
-      <c r="P23" s="61"/>
-      <c r="Q23" s="61"/>
-      <c r="R23" s="61"/>
-      <c r="S23" s="61"/>
-      <c r="T23" s="61"/>
-      <c r="U23" s="61"/>
-      <c r="V23" s="61"/>
-      <c r="W23" s="61"/>
-      <c r="X23" s="61"/>
-      <c r="Y23" s="61"/>
-      <c r="Z23" s="61"/>
-      <c r="AA23" s="61"/>
-      <c r="AB23" s="62"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="66"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="66"/>
+      <c r="O23" s="66"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="66"/>
+      <c r="U23" s="66"/>
+      <c r="V23" s="66"/>
+      <c r="W23" s="66"/>
+      <c r="X23" s="66"/>
+      <c r="Y23" s="66"/>
+      <c r="Z23" s="66"/>
+      <c r="AA23" s="66"/>
+      <c r="AB23" s="67"/>
     </row>
     <row r="24" spans="1:28" s="4" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="73" t="s">
+      <c r="B24" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="73" t="s">
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="73"/>
-      <c r="K24" s="73"/>
-      <c r="L24" s="44" t="s">
+      <c r="J24" s="68"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="M24" s="44"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="44"/>
-      <c r="P24" s="44"/>
-      <c r="Q24" s="44"/>
-      <c r="R24" s="9" t="s">
+      <c r="M24" s="70"/>
+      <c r="N24" s="70"/>
+      <c r="O24" s="70"/>
+      <c r="P24" s="70"/>
+      <c r="Q24" s="70"/>
+      <c r="R24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="S24" s="73" t="s">
+      <c r="S24" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="T24" s="73"/>
-      <c r="U24" s="73"/>
-      <c r="V24" s="73"/>
-      <c r="W24" s="75" t="s">
+      <c r="T24" s="68"/>
+      <c r="U24" s="68"/>
+      <c r="V24" s="68"/>
+      <c r="W24" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="X24" s="76"/>
-      <c r="Y24" s="73" t="s">
+      <c r="X24" s="72"/>
+      <c r="Y24" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="Z24" s="74"/>
-      <c r="AA24" s="74"/>
-      <c r="AB24" s="13" t="s">
+      <c r="Z24" s="69"/>
+      <c r="AA24" s="69"/>
+      <c r="AB24" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3616,656 +3584,507 @@
       <c r="A25" s="1">
         <v>1</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="28"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="89"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="85"/>
+      <c r="L25" s="85"/>
+      <c r="M25" s="85"/>
+      <c r="N25" s="85"/>
+      <c r="O25" s="85"/>
+      <c r="P25" s="85"/>
+      <c r="Q25" s="85"/>
       <c r="R25" s="5"/>
-      <c r="S25" s="29"/>
-      <c r="T25" s="29"/>
-      <c r="U25" s="29"/>
-      <c r="V25" s="29"/>
-      <c r="W25" s="30"/>
-      <c r="X25" s="31"/>
-      <c r="Y25" s="32"/>
-      <c r="Z25" s="32"/>
-      <c r="AA25" s="32"/>
-      <c r="AB25" s="11"/>
+      <c r="S25" s="86"/>
+      <c r="T25" s="86"/>
+      <c r="U25" s="86"/>
+      <c r="V25" s="86"/>
+      <c r="W25" s="87"/>
+      <c r="X25" s="88"/>
+      <c r="Y25" s="56"/>
+      <c r="Z25" s="56"/>
+      <c r="AA25" s="56"/>
+      <c r="AB25" s="9"/>
     </row>
     <row r="26" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="29"/>
-      <c r="T26" s="29"/>
-      <c r="U26" s="29"/>
-      <c r="V26" s="29"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="31"/>
-      <c r="Y26" s="32"/>
-      <c r="Z26" s="32"/>
-      <c r="AA26" s="32"/>
-      <c r="AB26" s="11"/>
+      <c r="B26" s="89"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="89"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="85"/>
+      <c r="L26" s="85"/>
+      <c r="M26" s="85"/>
+      <c r="N26" s="85"/>
+      <c r="O26" s="85"/>
+      <c r="P26" s="85"/>
+      <c r="Q26" s="85"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="86"/>
+      <c r="T26" s="86"/>
+      <c r="U26" s="86"/>
+      <c r="V26" s="86"/>
+      <c r="W26" s="87"/>
+      <c r="X26" s="88"/>
+      <c r="Y26" s="56"/>
+      <c r="Z26" s="56"/>
+      <c r="AA26" s="56"/>
+      <c r="AB26" s="9"/>
     </row>
     <row r="27" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>3</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
-      <c r="O27" s="28"/>
-      <c r="P27" s="28"/>
-      <c r="Q27" s="28"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="29"/>
-      <c r="T27" s="29"/>
-      <c r="U27" s="29"/>
-      <c r="V27" s="29"/>
-      <c r="W27" s="30"/>
-      <c r="X27" s="31"/>
-      <c r="Y27" s="32"/>
-      <c r="Z27" s="32"/>
-      <c r="AA27" s="32"/>
-      <c r="AB27" s="11"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="85"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="85"/>
+      <c r="L27" s="85"/>
+      <c r="M27" s="85"/>
+      <c r="N27" s="85"/>
+      <c r="O27" s="85"/>
+      <c r="P27" s="85"/>
+      <c r="Q27" s="85"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="86"/>
+      <c r="T27" s="86"/>
+      <c r="U27" s="86"/>
+      <c r="V27" s="86"/>
+      <c r="W27" s="87"/>
+      <c r="X27" s="88"/>
+      <c r="Y27" s="56"/>
+      <c r="Z27" s="56"/>
+      <c r="AA27" s="56"/>
+      <c r="AB27" s="9"/>
     </row>
     <row r="28" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>4</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="28"/>
-      <c r="Q28" s="28"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="29"/>
-      <c r="T28" s="29"/>
-      <c r="U28" s="29"/>
-      <c r="V28" s="29"/>
-      <c r="W28" s="30"/>
-      <c r="X28" s="31"/>
-      <c r="Y28" s="32"/>
-      <c r="Z28" s="32"/>
-      <c r="AA28" s="32"/>
-      <c r="AB28" s="11"/>
+      <c r="B28" s="89"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="85"/>
+      <c r="L28" s="85"/>
+      <c r="M28" s="85"/>
+      <c r="N28" s="85"/>
+      <c r="O28" s="85"/>
+      <c r="P28" s="85"/>
+      <c r="Q28" s="85"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="86"/>
+      <c r="T28" s="86"/>
+      <c r="U28" s="86"/>
+      <c r="V28" s="86"/>
+      <c r="W28" s="87"/>
+      <c r="X28" s="88"/>
+      <c r="Y28" s="56"/>
+      <c r="Z28" s="56"/>
+      <c r="AA28" s="56"/>
+      <c r="AB28" s="9"/>
     </row>
     <row r="29" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>5</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
-      <c r="O29" s="28"/>
-      <c r="P29" s="28"/>
-      <c r="Q29" s="28"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="29"/>
-      <c r="T29" s="29"/>
-      <c r="U29" s="29"/>
-      <c r="V29" s="29"/>
-      <c r="W29" s="30"/>
-      <c r="X29" s="31"/>
-      <c r="Y29" s="32"/>
-      <c r="Z29" s="32"/>
-      <c r="AA29" s="32"/>
-      <c r="AB29" s="11"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="89"/>
+      <c r="I29" s="85"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="85"/>
+      <c r="L29" s="85"/>
+      <c r="M29" s="85"/>
+      <c r="N29" s="85"/>
+      <c r="O29" s="85"/>
+      <c r="P29" s="85"/>
+      <c r="Q29" s="85"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="86"/>
+      <c r="T29" s="86"/>
+      <c r="U29" s="86"/>
+      <c r="V29" s="86"/>
+      <c r="W29" s="87"/>
+      <c r="X29" s="88"/>
+      <c r="Y29" s="56"/>
+      <c r="Z29" s="56"/>
+      <c r="AA29" s="56"/>
+      <c r="AB29" s="9"/>
     </row>
     <row r="30" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>6</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
-      <c r="O30" s="28"/>
-      <c r="P30" s="28"/>
-      <c r="Q30" s="28"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="29"/>
-      <c r="T30" s="29"/>
-      <c r="U30" s="29"/>
-      <c r="V30" s="29"/>
-      <c r="W30" s="30"/>
-      <c r="X30" s="31"/>
-      <c r="Y30" s="32"/>
-      <c r="Z30" s="32"/>
-      <c r="AA30" s="32"/>
-      <c r="AB30" s="11"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="85"/>
+      <c r="J30" s="85"/>
+      <c r="K30" s="85"/>
+      <c r="L30" s="85"/>
+      <c r="M30" s="85"/>
+      <c r="N30" s="85"/>
+      <c r="O30" s="85"/>
+      <c r="P30" s="85"/>
+      <c r="Q30" s="85"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="86"/>
+      <c r="T30" s="86"/>
+      <c r="U30" s="86"/>
+      <c r="V30" s="86"/>
+      <c r="W30" s="87"/>
+      <c r="X30" s="88"/>
+      <c r="Y30" s="56"/>
+      <c r="Z30" s="56"/>
+      <c r="AA30" s="56"/>
+      <c r="AB30" s="9"/>
     </row>
     <row r="31" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>7</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="28"/>
-      <c r="O31" s="28"/>
-      <c r="P31" s="28"/>
-      <c r="Q31" s="28"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="89"/>
+      <c r="I31" s="85"/>
+      <c r="J31" s="85"/>
+      <c r="K31" s="85"/>
+      <c r="L31" s="85"/>
+      <c r="M31" s="85"/>
+      <c r="N31" s="85"/>
+      <c r="O31" s="85"/>
+      <c r="P31" s="85"/>
+      <c r="Q31" s="85"/>
       <c r="R31" s="5"/>
-      <c r="S31" s="29"/>
-      <c r="T31" s="29"/>
-      <c r="U31" s="29"/>
-      <c r="V31" s="29"/>
-      <c r="W31" s="30"/>
-      <c r="X31" s="31"/>
-      <c r="Y31" s="32"/>
-      <c r="Z31" s="32"/>
-      <c r="AA31" s="32"/>
-      <c r="AB31" s="11"/>
+      <c r="S31" s="86"/>
+      <c r="T31" s="86"/>
+      <c r="U31" s="86"/>
+      <c r="V31" s="86"/>
+      <c r="W31" s="87"/>
+      <c r="X31" s="88"/>
+      <c r="Y31" s="56"/>
+      <c r="Z31" s="56"/>
+      <c r="AA31" s="56"/>
+      <c r="AB31" s="9"/>
     </row>
     <row r="32" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>8</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="28"/>
-      <c r="O32" s="28"/>
-      <c r="P32" s="28"/>
-      <c r="Q32" s="28"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="89"/>
+      <c r="G32" s="89"/>
+      <c r="H32" s="89"/>
+      <c r="I32" s="85"/>
+      <c r="J32" s="85"/>
+      <c r="K32" s="85"/>
+      <c r="L32" s="85"/>
+      <c r="M32" s="85"/>
+      <c r="N32" s="85"/>
+      <c r="O32" s="85"/>
+      <c r="P32" s="85"/>
+      <c r="Q32" s="85"/>
       <c r="R32" s="5"/>
-      <c r="S32" s="29"/>
-      <c r="T32" s="29"/>
-      <c r="U32" s="29"/>
-      <c r="V32" s="29"/>
-      <c r="W32" s="30"/>
-      <c r="X32" s="31"/>
-      <c r="Y32" s="32"/>
-      <c r="Z32" s="32"/>
-      <c r="AA32" s="32"/>
-      <c r="AB32" s="11"/>
+      <c r="S32" s="86"/>
+      <c r="T32" s="86"/>
+      <c r="U32" s="86"/>
+      <c r="V32" s="86"/>
+      <c r="W32" s="87"/>
+      <c r="X32" s="88"/>
+      <c r="Y32" s="56"/>
+      <c r="Z32" s="56"/>
+      <c r="AA32" s="56"/>
+      <c r="AB32" s="9"/>
     </row>
-    <row r="33" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>9</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="28"/>
-      <c r="O33" s="28"/>
-      <c r="P33" s="28"/>
-      <c r="Q33" s="28"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="89"/>
+      <c r="H33" s="89"/>
+      <c r="I33" s="85"/>
+      <c r="J33" s="85"/>
+      <c r="K33" s="85"/>
+      <c r="L33" s="85"/>
+      <c r="M33" s="85"/>
+      <c r="N33" s="85"/>
+      <c r="O33" s="85"/>
+      <c r="P33" s="85"/>
+      <c r="Q33" s="85"/>
       <c r="R33" s="5"/>
-      <c r="S33" s="29"/>
-      <c r="T33" s="29"/>
-      <c r="U33" s="29"/>
-      <c r="V33" s="29"/>
-      <c r="W33" s="30"/>
-      <c r="X33" s="31"/>
-      <c r="Y33" s="32"/>
-      <c r="Z33" s="32"/>
-      <c r="AA33" s="32"/>
-      <c r="AB33" s="11"/>
+      <c r="S33" s="86"/>
+      <c r="T33" s="86"/>
+      <c r="U33" s="86"/>
+      <c r="V33" s="86"/>
+      <c r="W33" s="87"/>
+      <c r="X33" s="88"/>
+      <c r="Y33" s="56"/>
+      <c r="Z33" s="56"/>
+      <c r="AA33" s="56"/>
+      <c r="AB33" s="9"/>
     </row>
-    <row r="34" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>10</v>
-      </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
-      <c r="N34" s="28"/>
-      <c r="O34" s="28"/>
-      <c r="P34" s="28"/>
-      <c r="Q34" s="28"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="29"/>
-      <c r="T34" s="29"/>
-      <c r="U34" s="29"/>
-      <c r="V34" s="29"/>
-      <c r="W34" s="30"/>
-      <c r="X34" s="31"/>
-      <c r="Y34" s="32"/>
-      <c r="Z34" s="32"/>
-      <c r="AA34" s="32"/>
-      <c r="AB34" s="11"/>
+    <row r="34" spans="1:31" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="91" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="92"/>
+      <c r="C34" s="92"/>
+      <c r="D34" s="92"/>
+      <c r="E34" s="92"/>
+      <c r="F34" s="93" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="93"/>
+      <c r="H34" s="93"/>
+      <c r="I34" s="93"/>
+      <c r="J34" s="93"/>
+      <c r="K34" s="93"/>
+      <c r="L34" s="93"/>
+      <c r="M34" s="93"/>
+      <c r="N34" s="93"/>
+      <c r="O34" s="93"/>
+      <c r="P34" s="66" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q34" s="66"/>
+      <c r="R34" s="66"/>
+      <c r="S34" s="66"/>
+      <c r="T34" s="66"/>
+      <c r="U34" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="V34" s="66"/>
+      <c r="W34" s="66"/>
+      <c r="X34" s="66"/>
+      <c r="Y34" s="66"/>
+      <c r="Z34" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA34" s="66"/>
+      <c r="AB34" s="67"/>
+      <c r="AC34" s="4"/>
     </row>
-    <row r="35" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>11</v>
-      </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
-      <c r="L35" s="28"/>
-      <c r="M35" s="28"/>
-      <c r="N35" s="28"/>
-      <c r="O35" s="28"/>
-      <c r="P35" s="28"/>
-      <c r="Q35" s="28"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="29"/>
-      <c r="T35" s="29"/>
-      <c r="U35" s="29"/>
-      <c r="V35" s="29"/>
-      <c r="W35" s="30"/>
-      <c r="X35" s="31"/>
-      <c r="Y35" s="32"/>
-      <c r="Z35" s="32"/>
-      <c r="AA35" s="32"/>
-      <c r="AB35" s="11"/>
+    <row r="35" spans="1:31" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="94" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="95"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="85"/>
+      <c r="I35" s="85"/>
+      <c r="J35" s="85"/>
+      <c r="K35" s="85"/>
+      <c r="L35" s="85"/>
+      <c r="M35" s="85"/>
+      <c r="N35" s="85"/>
+      <c r="O35" s="85"/>
+      <c r="P35" s="87"/>
+      <c r="Q35" s="129"/>
+      <c r="R35" s="129"/>
+      <c r="S35" s="129"/>
+      <c r="T35" s="88"/>
+      <c r="U35" s="87"/>
+      <c r="V35" s="129"/>
+      <c r="W35" s="129"/>
+      <c r="X35" s="129"/>
+      <c r="Y35" s="88"/>
+      <c r="Z35" s="85"/>
+      <c r="AA35" s="85"/>
+      <c r="AB35" s="130"/>
+      <c r="AD35" s="4"/>
     </row>
-    <row r="36" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>12</v>
-      </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="28"/>
-      <c r="N36" s="28"/>
-      <c r="O36" s="28"/>
-      <c r="P36" s="28"/>
-      <c r="Q36" s="28"/>
-      <c r="R36" s="5"/>
+    <row r="36" spans="1:31" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="95"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
+      <c r="Q36" s="29"/>
+      <c r="R36" s="29"/>
       <c r="S36" s="29"/>
       <c r="T36" s="29"/>
-      <c r="U36" s="29"/>
-      <c r="V36" s="29"/>
-      <c r="W36" s="30"/>
-      <c r="X36" s="31"/>
-      <c r="Y36" s="32"/>
-      <c r="Z36" s="32"/>
-      <c r="AA36" s="32"/>
-      <c r="AB36" s="11"/>
+      <c r="U36" s="85"/>
+      <c r="V36" s="85"/>
+      <c r="W36" s="85"/>
+      <c r="X36" s="85"/>
+      <c r="Y36" s="85"/>
+      <c r="Z36" s="85"/>
+      <c r="AA36" s="85"/>
+      <c r="AB36" s="130"/>
+      <c r="AE36" s="4"/>
     </row>
-    <row r="37" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>13</v>
-      </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
-      <c r="N37" s="28"/>
-      <c r="O37" s="28"/>
-      <c r="P37" s="28"/>
-      <c r="Q37" s="28"/>
-      <c r="R37" s="5"/>
+    <row r="37" spans="1:31" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="94" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="95"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="95"/>
+      <c r="E37" s="95"/>
+      <c r="F37" s="131"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="131"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
       <c r="S37" s="29"/>
       <c r="T37" s="29"/>
-      <c r="U37" s="29"/>
-      <c r="V37" s="29"/>
-      <c r="W37" s="30"/>
-      <c r="X37" s="31"/>
-      <c r="Y37" s="32"/>
-      <c r="Z37" s="32"/>
-      <c r="AA37" s="32"/>
-      <c r="AB37" s="11"/>
+      <c r="U37" s="132"/>
+      <c r="V37" s="85"/>
+      <c r="W37" s="85"/>
+      <c r="X37" s="85"/>
+      <c r="Y37" s="85"/>
+      <c r="Z37" s="85"/>
+      <c r="AA37" s="85"/>
+      <c r="AB37" s="130"/>
     </row>
-    <row r="38" spans="1:28" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
-        <v>14</v>
-      </c>
-      <c r="B38" s="66"/>
-      <c r="C38" s="66"/>
-      <c r="D38" s="66"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="66"/>
-      <c r="G38" s="66"/>
-      <c r="H38" s="66"/>
-      <c r="I38" s="67"/>
-      <c r="J38" s="67"/>
-      <c r="K38" s="67"/>
-      <c r="L38" s="67"/>
-      <c r="M38" s="67"/>
-      <c r="N38" s="67"/>
-      <c r="O38" s="67"/>
-      <c r="P38" s="67"/>
-      <c r="Q38" s="67"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="68"/>
-      <c r="T38" s="68"/>
-      <c r="U38" s="68"/>
-      <c r="V38" s="68"/>
-      <c r="W38" s="69"/>
-      <c r="X38" s="70"/>
-      <c r="Y38" s="71"/>
-      <c r="Z38" s="71"/>
-      <c r="AA38" s="71"/>
-      <c r="AB38" s="12"/>
+    <row r="38" spans="1:31" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="98" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="99"/>
+      <c r="C38" s="99"/>
+      <c r="D38" s="99"/>
+      <c r="E38" s="99"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="90"/>
+      <c r="H38" s="90"/>
+      <c r="I38" s="90"/>
+      <c r="J38" s="90"/>
+      <c r="K38" s="90"/>
+      <c r="L38" s="90"/>
+      <c r="M38" s="90"/>
+      <c r="N38" s="90"/>
+      <c r="O38" s="90"/>
+      <c r="P38" s="90"/>
+      <c r="Q38" s="90"/>
+      <c r="R38" s="90"/>
+      <c r="S38" s="90"/>
+      <c r="T38" s="90"/>
+      <c r="U38" s="90"/>
+      <c r="V38" s="90"/>
+      <c r="W38" s="90"/>
+      <c r="X38" s="90"/>
+      <c r="Y38" s="90"/>
+      <c r="Z38" s="90"/>
+      <c r="AA38" s="90"/>
+      <c r="AB38" s="133"/>
     </row>
-    <row r="39" spans="1:28" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" s="59"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="59"/>
-      <c r="E39" s="59"/>
-      <c r="F39" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="G39" s="60"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="60"/>
-      <c r="K39" s="60"/>
-      <c r="L39" s="60"/>
-      <c r="M39" s="60"/>
-      <c r="N39" s="60"/>
-      <c r="O39" s="60"/>
-      <c r="P39" s="61" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q39" s="61"/>
-      <c r="R39" s="61"/>
-      <c r="S39" s="61"/>
-      <c r="T39" s="61"/>
-      <c r="U39" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="V39" s="61"/>
-      <c r="W39" s="61"/>
-      <c r="X39" s="61"/>
-      <c r="Y39" s="61"/>
-      <c r="Z39" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA39" s="61"/>
-      <c r="AB39" s="62"/>
+    <row r="39" spans="1:31" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="96" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="97"/>
+      <c r="C39" s="97"/>
+      <c r="D39" s="97"/>
+      <c r="E39" s="97"/>
+      <c r="F39" s="97"/>
+      <c r="G39" s="97"/>
+      <c r="H39" s="97"/>
+      <c r="I39" s="97"/>
+      <c r="J39" s="97"/>
+      <c r="K39" s="97"/>
+      <c r="L39" s="97"/>
+      <c r="M39" s="97"/>
+      <c r="N39" s="97"/>
+      <c r="O39" s="97"/>
+      <c r="P39" s="97"/>
+      <c r="Q39" s="97"/>
+      <c r="R39" s="97"/>
+      <c r="S39" s="97"/>
+      <c r="T39" s="97"/>
+      <c r="U39" s="97"/>
+      <c r="V39" s="97"/>
+      <c r="W39" s="97"/>
+      <c r="X39" s="97"/>
+      <c r="Y39" s="97"/>
+      <c r="Z39" s="97"/>
+      <c r="AA39" s="97"/>
+      <c r="AB39" s="97"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="2"/>
     </row>
-    <row r="40" spans="1:28" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="52"/>
-      <c r="C40" s="52"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="54"/>
-      <c r="H40" s="54"/>
-      <c r="I40" s="54"/>
-      <c r="J40" s="54"/>
-      <c r="K40" s="54"/>
-      <c r="L40" s="54"/>
-      <c r="M40" s="54"/>
-      <c r="N40" s="54"/>
-      <c r="O40" s="54"/>
-      <c r="P40" s="63"/>
-      <c r="Q40" s="64"/>
-      <c r="R40" s="64"/>
-      <c r="S40" s="64"/>
-      <c r="T40" s="65"/>
-      <c r="U40" s="63"/>
-      <c r="V40" s="64"/>
-      <c r="W40" s="64"/>
-      <c r="X40" s="64"/>
-      <c r="Y40" s="65"/>
-      <c r="Z40" s="54"/>
-      <c r="AA40" s="54"/>
-      <c r="AB40" s="55"/>
+    <row r="40" spans="1:31" ht="25.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:31" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K41" s="3"/>
     </row>
-    <row r="41" spans="1:28" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="52"/>
-      <c r="C41" s="52"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="53"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="53"/>
-      <c r="I41" s="53"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="53"/>
-      <c r="L41" s="53"/>
-      <c r="M41" s="53"/>
-      <c r="N41" s="53"/>
-      <c r="O41" s="53"/>
-      <c r="P41" s="53"/>
-      <c r="Q41" s="53"/>
-      <c r="R41" s="53"/>
-      <c r="S41" s="53"/>
-      <c r="T41" s="53"/>
-      <c r="U41" s="54"/>
-      <c r="V41" s="54"/>
-      <c r="W41" s="54"/>
-      <c r="X41" s="54"/>
-      <c r="Y41" s="54"/>
-      <c r="Z41" s="54"/>
-      <c r="AA41" s="54"/>
-      <c r="AB41" s="55"/>
-    </row>
-    <row r="42" spans="1:28" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="52"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="53"/>
-      <c r="M42" s="53"/>
-      <c r="N42" s="53"/>
-      <c r="O42" s="53"/>
-      <c r="P42" s="56"/>
-      <c r="Q42" s="53"/>
-      <c r="R42" s="53"/>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
-      <c r="U42" s="57"/>
-      <c r="V42" s="54"/>
-      <c r="W42" s="54"/>
-      <c r="X42" s="54"/>
-      <c r="Y42" s="54"/>
-      <c r="Z42" s="54"/>
-      <c r="AA42" s="54"/>
-      <c r="AB42" s="55"/>
-    </row>
-    <row r="43" spans="1:28" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
-      <c r="K43" s="49"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="49"/>
-      <c r="N43" s="49"/>
-      <c r="O43" s="49"/>
-      <c r="P43" s="49"/>
-      <c r="Q43" s="49"/>
-      <c r="R43" s="49"/>
-      <c r="S43" s="49"/>
-      <c r="T43" s="49"/>
-      <c r="U43" s="49"/>
-      <c r="V43" s="49"/>
-      <c r="W43" s="49"/>
-      <c r="X43" s="49"/>
-      <c r="Y43" s="49"/>
-      <c r="Z43" s="49"/>
-      <c r="AA43" s="49"/>
-      <c r="AB43" s="50"/>
-    </row>
-    <row r="44" spans="1:28" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="43"/>
-      <c r="L44" s="43"/>
-      <c r="M44" s="43"/>
-      <c r="N44" s="43"/>
-      <c r="O44" s="43"/>
-      <c r="P44" s="43"/>
-      <c r="Q44" s="43"/>
-      <c r="R44" s="43"/>
-      <c r="S44" s="43"/>
-      <c r="T44" s="43"/>
-      <c r="U44" s="43"/>
-      <c r="V44" s="43"/>
-      <c r="W44" s="43"/>
-      <c r="X44" s="43"/>
-      <c r="Y44" s="43"/>
-      <c r="Z44" s="43"/>
-      <c r="AA44" s="43"/>
-      <c r="AB44" s="43"/>
-    </row>
-    <row r="45" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K46" s="3"/>
-    </row>
-    <row r="47" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:28" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:31" ht="25.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:31" ht="57.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:31" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:31" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:31" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:31" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:31" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="21.6" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4648,161 +4467,31 @@
     <row r="428" ht="2.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="429" ht="2.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="202">
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="H1:AB1"/>
-    <mergeCell ref="H2:AB2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:P3"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="T3:W3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:P5"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="X5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:P4"/>
-    <mergeCell ref="Q4:S4"/>
-    <mergeCell ref="T4:W4"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="T7:W7"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:P6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="T6:W6"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="K11:P11"/>
-    <mergeCell ref="Q11:V11"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="K10:P10"/>
-    <mergeCell ref="Q10:V10"/>
-    <mergeCell ref="A8:AB8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="K9:P9"/>
-    <mergeCell ref="Q9:V9"/>
-    <mergeCell ref="W9:Y9"/>
-    <mergeCell ref="Z9:AB9"/>
-    <mergeCell ref="S18:AB18"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="S19:AB19"/>
-    <mergeCell ref="A15:G19"/>
-    <mergeCell ref="H15:P19"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="S16:AB16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="S17:AB17"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="Q15:AB15"/>
-    <mergeCell ref="A23:AB23"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="L24:Q24"/>
-    <mergeCell ref="S24:V24"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="Y24:AA24"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="H20:AB20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="H21:AB21"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="H22:AB22"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="L26:Q26"/>
-    <mergeCell ref="S26:V26"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="Y26:AA26"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="L25:Q25"/>
-    <mergeCell ref="S25:V25"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="Y25:AA25"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="L36:Q36"/>
-    <mergeCell ref="S36:V36"/>
-    <mergeCell ref="W36:X36"/>
-    <mergeCell ref="Y36:AA36"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="L33:Q33"/>
-    <mergeCell ref="S33:V33"/>
-    <mergeCell ref="W33:X33"/>
-    <mergeCell ref="Y33:AA33"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="L35:Q35"/>
-    <mergeCell ref="S35:V35"/>
-    <mergeCell ref="W35:X35"/>
-    <mergeCell ref="Y35:AA35"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:Q34"/>
-    <mergeCell ref="S34:V34"/>
-    <mergeCell ref="W34:X34"/>
-    <mergeCell ref="Y34:AA34"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="L38:Q38"/>
-    <mergeCell ref="S38:V38"/>
-    <mergeCell ref="W38:X38"/>
-    <mergeCell ref="Y38:AA38"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="L37:Q37"/>
-    <mergeCell ref="S37:V37"/>
-    <mergeCell ref="W37:X37"/>
-    <mergeCell ref="Y37:AA37"/>
-    <mergeCell ref="Z42:AB42"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="F39:O39"/>
-    <mergeCell ref="P39:T39"/>
-    <mergeCell ref="U39:Y39"/>
-    <mergeCell ref="Z39:AB39"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="F40:O40"/>
-    <mergeCell ref="P40:T40"/>
-    <mergeCell ref="U40:Y40"/>
-    <mergeCell ref="Z40:AB40"/>
-    <mergeCell ref="W27:X27"/>
-    <mergeCell ref="Y27:AA27"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="A44:AB44"/>
-    <mergeCell ref="W10:Y11"/>
-    <mergeCell ref="Z10:AB11"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="E13:J13"/>
-    <mergeCell ref="K13:P13"/>
-    <mergeCell ref="Q13:V13"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="F43:O43"/>
-    <mergeCell ref="P43:T43"/>
-    <mergeCell ref="U43:Y43"/>
-    <mergeCell ref="Z43:AB43"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="F41:O41"/>
-    <mergeCell ref="P41:T41"/>
-    <mergeCell ref="U41:Y41"/>
-    <mergeCell ref="Z41:AB41"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="F42:O42"/>
-    <mergeCell ref="P42:T42"/>
-    <mergeCell ref="U42:Y42"/>
+  <mergeCells count="172">
+    <mergeCell ref="W13:Y13"/>
+    <mergeCell ref="W14:Y14"/>
+    <mergeCell ref="Z13:AB13"/>
+    <mergeCell ref="Z14:AB14"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="L32:Q32"/>
+    <mergeCell ref="S32:V32"/>
+    <mergeCell ref="W32:X32"/>
+    <mergeCell ref="Y32:AA32"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="L31:Q31"/>
+    <mergeCell ref="S31:V31"/>
+    <mergeCell ref="W31:X31"/>
+    <mergeCell ref="Y31:AA31"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="L30:Q30"/>
+    <mergeCell ref="S30:V30"/>
+    <mergeCell ref="W30:X30"/>
+    <mergeCell ref="Y30:AA30"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="I29:K29"/>
     <mergeCell ref="L29:Q29"/>
     <mergeCell ref="S29:V29"/>
     <mergeCell ref="W29:X29"/>
@@ -4827,30 +4516,130 @@
     <mergeCell ref="I27:K27"/>
     <mergeCell ref="L27:Q27"/>
     <mergeCell ref="S27:V27"/>
-    <mergeCell ref="W13:Y13"/>
-    <mergeCell ref="W14:Y14"/>
-    <mergeCell ref="Z13:AB13"/>
-    <mergeCell ref="Z14:AB14"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="L32:Q32"/>
-    <mergeCell ref="S32:V32"/>
-    <mergeCell ref="W32:X32"/>
-    <mergeCell ref="Y32:AA32"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="L31:Q31"/>
-    <mergeCell ref="S31:V31"/>
-    <mergeCell ref="W31:X31"/>
-    <mergeCell ref="Y31:AA31"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="L30:Q30"/>
-    <mergeCell ref="S30:V30"/>
-    <mergeCell ref="W30:X30"/>
-    <mergeCell ref="Y30:AA30"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="W27:X27"/>
+    <mergeCell ref="Y27:AA27"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="A39:AB39"/>
+    <mergeCell ref="W10:Y11"/>
+    <mergeCell ref="Z10:AB11"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="E13:J13"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="Q13:V13"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="F38:O38"/>
+    <mergeCell ref="P38:T38"/>
+    <mergeCell ref="U38:Y38"/>
+    <mergeCell ref="Z38:AB38"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="F36:O36"/>
+    <mergeCell ref="P36:T36"/>
+    <mergeCell ref="U36:Y36"/>
+    <mergeCell ref="Z36:AB36"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="F37:O37"/>
+    <mergeCell ref="P37:T37"/>
+    <mergeCell ref="U37:Y37"/>
+    <mergeCell ref="Z37:AB37"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="F34:O34"/>
+    <mergeCell ref="P34:T34"/>
+    <mergeCell ref="U34:Y34"/>
+    <mergeCell ref="Z34:AB34"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="F35:O35"/>
+    <mergeCell ref="P35:T35"/>
+    <mergeCell ref="U35:Y35"/>
+    <mergeCell ref="Z35:AB35"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="L33:Q33"/>
+    <mergeCell ref="S33:V33"/>
+    <mergeCell ref="W33:X33"/>
+    <mergeCell ref="Y33:AA33"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="L26:Q26"/>
+    <mergeCell ref="S26:V26"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="Y26:AA26"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="L25:Q25"/>
+    <mergeCell ref="S25:V25"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="Y25:AA25"/>
+    <mergeCell ref="A23:AB23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="L24:Q24"/>
+    <mergeCell ref="S24:V24"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="Y24:AA24"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="H20:AB20"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="H21:AB21"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="H22:AB22"/>
+    <mergeCell ref="S18:AB18"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="S19:AB19"/>
+    <mergeCell ref="A15:G19"/>
+    <mergeCell ref="H15:P19"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="S16:AB16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="S17:AB17"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="Q15:AB15"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="K11:P11"/>
+    <mergeCell ref="Q11:V11"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="K10:P10"/>
+    <mergeCell ref="Q10:V10"/>
+    <mergeCell ref="A8:AB8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="K9:P9"/>
+    <mergeCell ref="Q9:V9"/>
+    <mergeCell ref="W9:Y9"/>
+    <mergeCell ref="Z9:AB9"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:P7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="T6:W6"/>
+    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:P5"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="X5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="T4:W4"/>
+    <mergeCell ref="X4:Z4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="H1:AB1"/>
+    <mergeCell ref="H2:AB2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="AA3:AB3"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0" top="0.27559055118110237" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4871,8 +4660,8 @@
                     <xdr:rowOff>161925</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>257175</xdr:colOff>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </to>
@@ -4893,8 +4682,8 @@
                     <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>15</xdr:col>
-                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:col>16</xdr:col>
+                    <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>133350</xdr:rowOff>
                   </to>

</xml_diff>